<commit_message>
add basic xlsx support
</commit_message>
<xml_diff>
--- a/resources/test.xlsx
+++ b/resources/test.xlsx
@@ -6,19 +6,22 @@
     <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Иван1</t>
   </si>
   <si>
     <t>Тверь</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
   <si>
     <t>Иван2</t>
@@ -140,7 +143,8 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
@@ -650,7 +654,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0" zoomScale="100">
+    <sheetView topLeftCell="A17" workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -663,243 +667,333 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>1</v>
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>1</v>
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>1</v>
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>1</v>
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>1</v>
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>1</v>
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>1</v>
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>1</v>
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>1</v>
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>1</v>
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>1</v>
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>1</v>
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1</v>
+      <c r="A18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>1</v>
+      <c r="A19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>1</v>
+      <c r="A20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>1</v>
+      <c r="A21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>1</v>
+      <c r="A22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>1</v>
+      <c r="A23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>1</v>
+      <c r="A24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>1</v>
+      <c r="A25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>1</v>
+      <c r="A26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>1</v>
+      <c r="A27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>1</v>
+      <c r="A28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>1</v>
+      <c r="A29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>1</v>
+      <c r="A30" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>